<commit_message>
Fixed stop process button when process finishes
</commit_message>
<xml_diff>
--- a/Arquivo de Mensagens/Arquivo de mensagens.xlsx
+++ b/Arquivo de Mensagens/Arquivo de mensagens.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Customer Messages Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHubPersonal\SendWhatsAppMessages\Arquivo de Mensagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC813D9-576C-45D8-8446-67DBC1DDF4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09C0347-5D85-42C4-9BC1-78B8561CF30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{569289BC-D768-472D-9366-0DDE05FEA49D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Pablo</t>
   </si>
@@ -558,7 +558,7 @@
   <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,9 +601,7 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="3" t="str">
         <f>"Testing Message for "&amp;A3</f>
         <v>Testing Message for Pedro with valid message</v>
@@ -638,9 +636,7 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="3" t="str">
         <f>"Testing Message for "&amp;A6</f>
         <v>Testing Message for José valid message</v>
@@ -650,9 +646,6 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C7" s="3" t="str">
         <f>"Testing Message for "&amp;A7</f>
         <v>Testing Message for José wrong number</v>
@@ -662,27 +655,18 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C10" s="3" t="str">
         <f>"Testing Message for "&amp;A10</f>
         <v>Testing Message for Maria with message</v>
@@ -701,9 +685,7 @@
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="3" t="str">
         <f>"Testing Message for "&amp;A12</f>
         <v>Testing Message for João message</v>
@@ -721,9 +703,6 @@
     <row r="14" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>"A very long text message with a link here for "&amp;A14&amp;"
@@ -736,9 +715,6 @@
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C15" s="4" t="str">
         <f>"A very long text message with a link here for "&amp;A15&amp;"
  https://www.google.com/"</f>
@@ -751,9 +727,6 @@
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C16" s="3" t="str">
         <f>"Testing Message for "&amp;A16</f>
         <v>Testing Message for Beltrano</v>
@@ -763,9 +736,6 @@
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C17" s="3" t="str">
         <f>"Testing Message for "&amp;A17</f>
         <v>Testing Message for Sultano</v>
@@ -776,9 +746,7 @@
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="4" t="str">
         <f>"A very long text message with a link here for "&amp;A18&amp;"
  https://www.instagram.com/"</f>

</xml_diff>